<commit_message>
add xls esita config
</commit_message>
<xml_diff>
--- a/MBUTYcap/config/MB.ESTIA_achitecture.xlsx
+++ b/MBUTYcap/config/MB.ESTIA_achitecture.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescopiscitelli/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescopiscitelli/Documents/PYTHON/MBUTYcap/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00E6439-F348-144E-9B78-79202B016302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DAEFA0-2B59-094C-9261-6E9E09B4EA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="500" windowWidth="37640" windowHeight="24640" activeTab="1" xr2:uid="{C1E7998F-7E5B-614C-9EEF-0F74FEBFC573}"/>
+    <workbookView xWindow="-1440" yWindow="-28300" windowWidth="36780" windowHeight="25260" activeTab="2" xr2:uid="{C1E7998F-7E5B-614C-9EEF-0F74FEBFC573}"/>
   </bookViews>
   <sheets>
     <sheet name="SectorsRings" sheetId="1" r:id="rId1"/>
     <sheet name="Channels" sheetId="2" r:id="rId2"/>
+    <sheet name="WireToCassette" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t xml:space="preserve">Cassette </t>
   </si>
@@ -70,12 +71,22 @@
   <si>
     <t>front wire</t>
   </si>
+  <si>
+    <t>Wire 
+pixel number 
+min</t>
+  </si>
+  <si>
+    <t>Wire 
+pixel number 
+max</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -97,6 +108,19 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Avenir Book"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -180,22 +204,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,919 +545,897 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{458F06AE-EC8C-8643-ABE3-691D5B79DF97}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="6.1640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="4.83203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="5" style="2" customWidth="1"/>
-    <col min="7" max="8" width="10.83203125" style="2"/>
-    <col min="9" max="9" width="1.83203125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="6.1640625" style="4"/>
+    <col min="2" max="2" width="7" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="6.1640625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="14" t="s">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="A3" s="8">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>0</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="A4" s="8">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>0</v>
-      </c>
-      <c r="B5" s="4">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="A5" s="8">
+        <v>0</v>
+      </c>
+      <c r="B5" s="9">
+        <v>2</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>0</v>
-      </c>
-      <c r="B6" s="4">
-        <v>3</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="A6" s="8">
+        <v>0</v>
+      </c>
+      <c r="B6" s="9">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>0</v>
-      </c>
-      <c r="B7" s="4">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="A7" s="8">
+        <v>0</v>
+      </c>
+      <c r="B7" s="9">
+        <v>4</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>0</v>
-      </c>
-      <c r="B8" s="5">
+      <c r="A8" s="8">
+        <v>0</v>
+      </c>
+      <c r="B8" s="10">
         <v>5</v>
       </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0</v>
-      </c>
-      <c r="E8" s="5">
+      <c r="C8" s="10">
+        <v>1</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+      <c r="E8" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>0</v>
-      </c>
-      <c r="B9" s="5">
+      <c r="A9" s="8">
+        <v>0</v>
+      </c>
+      <c r="B9" s="10">
         <v>6</v>
       </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5">
+      <c r="C9" s="10">
+        <v>1</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+      <c r="E9" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>0</v>
-      </c>
-      <c r="B10" s="5">
+      <c r="A10" s="8">
+        <v>0</v>
+      </c>
+      <c r="B10" s="10">
         <v>7</v>
       </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="C10" s="10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>1</v>
-      </c>
-      <c r="B12" s="5">
+      <c r="A12" s="11">
+        <v>1</v>
+      </c>
+      <c r="B12" s="10">
         <v>8</v>
       </c>
-      <c r="C12" s="5">
-        <v>1</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0</v>
-      </c>
-      <c r="E12" s="5">
+      <c r="C12" s="10">
+        <v>1</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+      <c r="E12" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>1</v>
-      </c>
-      <c r="B13" s="5">
+      <c r="A13" s="11">
+        <v>1</v>
+      </c>
+      <c r="B13" s="10">
         <v>9</v>
       </c>
-      <c r="C13" s="5">
-        <v>1</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0</v>
-      </c>
-      <c r="E13" s="5">
+      <c r="C13" s="10">
+        <v>1</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4">
+      <c r="A14" s="11">
+        <v>1</v>
+      </c>
+      <c r="B14" s="9">
         <v>10</v>
       </c>
-      <c r="C14" s="4">
-        <v>2</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0</v>
-      </c>
-      <c r="E14" s="4">
+      <c r="C14" s="9">
+        <v>2</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>1</v>
-      </c>
-      <c r="B15" s="4">
+      <c r="A15" s="11">
+        <v>1</v>
+      </c>
+      <c r="B15" s="9">
         <v>11</v>
       </c>
-      <c r="C15" s="4">
-        <v>2</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0</v>
-      </c>
-      <c r="E15" s="4">
+      <c r="C15" s="9">
+        <v>2</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0</v>
+      </c>
+      <c r="E15" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4">
+      <c r="A16" s="11">
+        <v>1</v>
+      </c>
+      <c r="B16" s="9">
         <v>12</v>
       </c>
-      <c r="C16" s="4">
-        <v>2</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-      <c r="E16" s="4">
+      <c r="C16" s="9">
+        <v>2</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0</v>
+      </c>
+      <c r="E16" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>1</v>
-      </c>
-      <c r="B17" s="4">
+      <c r="A17" s="11">
+        <v>1</v>
+      </c>
+      <c r="B17" s="9">
         <v>13</v>
       </c>
-      <c r="C17" s="4">
-        <v>2</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0</v>
-      </c>
-      <c r="E17" s="4">
+      <c r="C17" s="9">
+        <v>2</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>1</v>
-      </c>
-      <c r="B18" s="4">
+      <c r="A18" s="11">
+        <v>1</v>
+      </c>
+      <c r="B18" s="9">
         <v>14</v>
       </c>
-      <c r="C18" s="4">
-        <v>2</v>
-      </c>
-      <c r="D18" s="4">
-        <v>0</v>
-      </c>
-      <c r="E18" s="4">
+      <c r="C18" s="9">
+        <v>2</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0</v>
+      </c>
+      <c r="E18" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>1</v>
-      </c>
-      <c r="B19" s="5">
+      <c r="A19" s="11">
+        <v>1</v>
+      </c>
+      <c r="B19" s="10">
         <v>15</v>
       </c>
-      <c r="C19" s="5">
-        <v>3</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0</v>
-      </c>
-      <c r="E19" s="5">
+      <c r="C19" s="10">
+        <v>3</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0</v>
+      </c>
+      <c r="E19" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>2</v>
-      </c>
-      <c r="B21" s="5">
+      <c r="A21" s="8">
+        <v>2</v>
+      </c>
+      <c r="B21" s="10">
         <v>16</v>
       </c>
-      <c r="C21" s="5">
-        <v>3</v>
-      </c>
-      <c r="D21" s="5">
-        <v>0</v>
-      </c>
-      <c r="E21" s="5">
+      <c r="C21" s="10">
+        <v>3</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0</v>
+      </c>
+      <c r="E21" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>2</v>
-      </c>
-      <c r="B22" s="5">
+      <c r="A22" s="8">
+        <v>2</v>
+      </c>
+      <c r="B22" s="10">
         <v>17</v>
       </c>
-      <c r="C22" s="5">
-        <v>3</v>
-      </c>
-      <c r="D22" s="5">
-        <v>0</v>
-      </c>
-      <c r="E22" s="5">
+      <c r="C22" s="10">
+        <v>3</v>
+      </c>
+      <c r="D22" s="10">
+        <v>0</v>
+      </c>
+      <c r="E22" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>2</v>
-      </c>
-      <c r="B23" s="5">
+      <c r="A23" s="8">
+        <v>2</v>
+      </c>
+      <c r="B23" s="10">
         <v>18</v>
       </c>
-      <c r="C23" s="5">
-        <v>3</v>
-      </c>
-      <c r="D23" s="5">
-        <v>0</v>
-      </c>
-      <c r="E23" s="5">
+      <c r="C23" s="10">
+        <v>3</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+      <c r="E23" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>2</v>
-      </c>
-      <c r="B24" s="5">
+      <c r="A24" s="8">
+        <v>2</v>
+      </c>
+      <c r="B24" s="10">
         <v>19</v>
       </c>
-      <c r="C24" s="5">
-        <v>3</v>
-      </c>
-      <c r="D24" s="5">
-        <v>0</v>
-      </c>
-      <c r="E24" s="5">
+      <c r="C24" s="10">
+        <v>3</v>
+      </c>
+      <c r="D24" s="10">
+        <v>0</v>
+      </c>
+      <c r="E24" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>2</v>
-      </c>
-      <c r="B25" s="4">
+      <c r="A25" s="8">
+        <v>2</v>
+      </c>
+      <c r="B25" s="9">
         <v>20</v>
       </c>
-      <c r="C25" s="4">
-        <v>4</v>
-      </c>
-      <c r="D25" s="4">
-        <v>0</v>
-      </c>
-      <c r="E25" s="4">
+      <c r="C25" s="9">
+        <v>4</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>2</v>
-      </c>
-      <c r="B26" s="4">
+      <c r="A26" s="8">
+        <v>2</v>
+      </c>
+      <c r="B26" s="9">
         <v>21</v>
       </c>
-      <c r="C26" s="4">
-        <v>4</v>
-      </c>
-      <c r="D26" s="4">
-        <v>0</v>
-      </c>
-      <c r="E26" s="4">
+      <c r="C26" s="9">
+        <v>4</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>2</v>
-      </c>
-      <c r="B27" s="4">
+      <c r="A27" s="8">
+        <v>2</v>
+      </c>
+      <c r="B27" s="9">
         <v>22</v>
       </c>
-      <c r="C27" s="4">
-        <v>4</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0</v>
-      </c>
-      <c r="E27" s="4">
+      <c r="C27" s="9">
+        <v>4</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>2</v>
-      </c>
-      <c r="B28" s="4">
+      <c r="A28" s="8">
+        <v>2</v>
+      </c>
+      <c r="B28" s="9">
         <v>23</v>
       </c>
-      <c r="C28" s="4">
-        <v>4</v>
-      </c>
-      <c r="D28" s="4">
-        <v>0</v>
-      </c>
-      <c r="E28" s="4">
+      <c r="C28" s="9">
+        <v>4</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0</v>
+      </c>
+      <c r="E28" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
-        <v>3</v>
-      </c>
-      <c r="B30" s="4">
+      <c r="A30" s="12">
+        <v>3</v>
+      </c>
+      <c r="B30" s="9">
         <v>24</v>
       </c>
-      <c r="C30" s="4">
-        <v>4</v>
-      </c>
-      <c r="D30" s="4">
-        <v>0</v>
-      </c>
-      <c r="E30" s="4">
+      <c r="C30" s="9">
+        <v>4</v>
+      </c>
+      <c r="D30" s="9">
+        <v>0</v>
+      </c>
+      <c r="E30" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
-        <v>3</v>
-      </c>
-      <c r="B31" s="5">
+      <c r="A31" s="12">
+        <v>3</v>
+      </c>
+      <c r="B31" s="10">
         <v>25</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="10">
         <v>5</v>
       </c>
-      <c r="D31" s="5">
-        <v>0</v>
-      </c>
-      <c r="E31" s="5">
+      <c r="D31" s="10">
+        <v>0</v>
+      </c>
+      <c r="E31" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
-        <v>3</v>
-      </c>
-      <c r="B32" s="5">
+      <c r="A32" s="12">
+        <v>3</v>
+      </c>
+      <c r="B32" s="10">
         <v>26</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="10">
         <v>5</v>
       </c>
-      <c r="D32" s="5">
-        <v>0</v>
-      </c>
-      <c r="E32" s="5">
+      <c r="D32" s="10">
+        <v>0</v>
+      </c>
+      <c r="E32" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
-        <v>3</v>
-      </c>
-      <c r="B33" s="5">
+      <c r="A33" s="12">
+        <v>3</v>
+      </c>
+      <c r="B33" s="10">
         <v>27</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="10">
         <v>5</v>
       </c>
-      <c r="D33" s="5">
-        <v>0</v>
-      </c>
-      <c r="E33" s="5">
+      <c r="D33" s="10">
+        <v>0</v>
+      </c>
+      <c r="E33" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
-        <v>3</v>
-      </c>
-      <c r="B34" s="5">
+      <c r="A34" s="12">
+        <v>3</v>
+      </c>
+      <c r="B34" s="10">
         <v>28</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="10">
         <v>5</v>
       </c>
-      <c r="D34" s="5">
-        <v>0</v>
-      </c>
-      <c r="E34" s="5">
+      <c r="D34" s="10">
+        <v>0</v>
+      </c>
+      <c r="E34" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
-        <v>3</v>
-      </c>
-      <c r="B35" s="5">
+      <c r="A35" s="12">
+        <v>3</v>
+      </c>
+      <c r="B35" s="10">
         <v>29</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="10">
         <v>5</v>
       </c>
-      <c r="D35" s="5">
-        <v>0</v>
-      </c>
-      <c r="E35" s="5">
+      <c r="D35" s="10">
+        <v>0</v>
+      </c>
+      <c r="E35" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
-        <v>3</v>
-      </c>
-      <c r="B36" s="4">
+      <c r="A36" s="12">
+        <v>3</v>
+      </c>
+      <c r="B36" s="9">
         <v>30</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="9">
         <v>6</v>
       </c>
-      <c r="D36" s="4">
-        <v>0</v>
-      </c>
-      <c r="E36" s="4">
+      <c r="D36" s="9">
+        <v>0</v>
+      </c>
+      <c r="E36" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
-        <v>3</v>
-      </c>
-      <c r="B37" s="4">
+      <c r="A37" s="12">
+        <v>3</v>
+      </c>
+      <c r="B37" s="9">
         <v>31</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="9">
         <v>6</v>
       </c>
-      <c r="D37" s="4">
-        <v>0</v>
-      </c>
-      <c r="E37" s="4">
+      <c r="D37" s="9">
+        <v>0</v>
+      </c>
+      <c r="E37" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
-        <v>4</v>
-      </c>
-      <c r="B39" s="4">
+      <c r="A39" s="8">
+        <v>4</v>
+      </c>
+      <c r="B39" s="9">
         <v>32</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="9">
         <v>6</v>
       </c>
-      <c r="D39" s="4">
-        <v>0</v>
-      </c>
-      <c r="E39" s="4">
+      <c r="D39" s="9">
+        <v>0</v>
+      </c>
+      <c r="E39" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>4</v>
-      </c>
-      <c r="B40" s="4">
+      <c r="A40" s="8">
+        <v>4</v>
+      </c>
+      <c r="B40" s="9">
         <v>33</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="9">
         <v>6</v>
       </c>
-      <c r="D40" s="4">
-        <v>0</v>
-      </c>
-      <c r="E40" s="4">
+      <c r="D40" s="9">
+        <v>0</v>
+      </c>
+      <c r="E40" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
-        <v>4</v>
-      </c>
-      <c r="B41" s="4">
+      <c r="A41" s="8">
+        <v>4</v>
+      </c>
+      <c r="B41" s="9">
         <v>34</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="9">
         <v>6</v>
       </c>
-      <c r="D41" s="4">
-        <v>0</v>
-      </c>
-      <c r="E41" s="4">
+      <c r="D41" s="9">
+        <v>0</v>
+      </c>
+      <c r="E41" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
-        <v>4</v>
-      </c>
-      <c r="B42" s="5">
+      <c r="A42" s="8">
+        <v>4</v>
+      </c>
+      <c r="B42" s="10">
         <v>35</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="10">
         <v>7</v>
       </c>
-      <c r="D42" s="5">
-        <v>0</v>
-      </c>
-      <c r="E42" s="5">
+      <c r="D42" s="10">
+        <v>0</v>
+      </c>
+      <c r="E42" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
-        <v>4</v>
-      </c>
-      <c r="B43" s="5">
+      <c r="A43" s="8">
+        <v>4</v>
+      </c>
+      <c r="B43" s="10">
         <v>36</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="10">
         <v>7</v>
       </c>
-      <c r="D43" s="5">
-        <v>0</v>
-      </c>
-      <c r="E43" s="5">
+      <c r="D43" s="10">
+        <v>0</v>
+      </c>
+      <c r="E43" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
-        <v>4</v>
-      </c>
-      <c r="B44" s="5">
+      <c r="A44" s="8">
+        <v>4</v>
+      </c>
+      <c r="B44" s="10">
         <v>37</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="10">
         <v>7</v>
       </c>
-      <c r="D44" s="5">
-        <v>0</v>
-      </c>
-      <c r="E44" s="5">
+      <c r="D44" s="10">
+        <v>0</v>
+      </c>
+      <c r="E44" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
-        <v>4</v>
-      </c>
-      <c r="B45" s="5">
+      <c r="A45" s="8">
+        <v>4</v>
+      </c>
+      <c r="B45" s="10">
         <v>38</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C45" s="10">
         <v>7</v>
       </c>
-      <c r="D45" s="5">
-        <v>0</v>
-      </c>
-      <c r="E45" s="5">
+      <c r="D45" s="10">
+        <v>0</v>
+      </c>
+      <c r="E45" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <v>4</v>
-      </c>
-      <c r="B46" s="5">
+      <c r="A46" s="8">
+        <v>4</v>
+      </c>
+      <c r="B46" s="10">
         <v>39</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="10">
         <v>7</v>
       </c>
-      <c r="D46" s="5">
-        <v>0</v>
-      </c>
-      <c r="E46" s="5">
+      <c r="D46" s="10">
+        <v>0</v>
+      </c>
+      <c r="E46" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="7">
+      <c r="A48" s="12">
         <v>5</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B48" s="9">
         <v>40</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C48" s="9">
         <v>8</v>
       </c>
-      <c r="D48" s="4">
-        <v>0</v>
-      </c>
-      <c r="E48" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="7">
+      <c r="D48" s="9">
+        <v>0</v>
+      </c>
+      <c r="E48" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="12">
         <v>5</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B49" s="9">
         <v>41</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49" s="9">
         <v>8</v>
       </c>
-      <c r="D49" s="4">
-        <v>0</v>
-      </c>
-      <c r="E49" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="7">
+      <c r="D49" s="9">
+        <v>0</v>
+      </c>
+      <c r="E49" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="12">
         <v>5</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B50" s="9">
         <v>42</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C50" s="9">
         <v>8</v>
       </c>
-      <c r="D50" s="4">
-        <v>0</v>
-      </c>
-      <c r="E50" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="7">
+      <c r="D50" s="9">
+        <v>0</v>
+      </c>
+      <c r="E50" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="12">
         <v>5</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B51" s="9">
         <v>43</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C51" s="9">
         <v>8</v>
       </c>
-      <c r="D51" s="4">
-        <v>0</v>
-      </c>
-      <c r="E51" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
+      <c r="D51" s="9">
+        <v>0</v>
+      </c>
+      <c r="E51" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="12">
         <v>5</v>
       </c>
-      <c r="B52" s="4">
+      <c r="B52" s="9">
         <v>44</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C52" s="9">
         <v>8</v>
       </c>
-      <c r="D52" s="4">
-        <v>0</v>
-      </c>
-      <c r="E52" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="7">
+      <c r="D52" s="9">
+        <v>0</v>
+      </c>
+      <c r="E52" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="12">
         <v>5</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B53" s="10">
         <v>45</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C53" s="10">
         <v>9</v>
       </c>
-      <c r="D53" s="5">
-        <v>0</v>
-      </c>
-      <c r="E53" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="7">
+      <c r="D53" s="10">
+        <v>0</v>
+      </c>
+      <c r="E53" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="12">
         <v>5</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B54" s="10">
         <v>46</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C54" s="10">
         <v>9</v>
       </c>
-      <c r="D54" s="5">
-        <v>0</v>
-      </c>
-      <c r="E54" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="7">
+      <c r="D54" s="10">
+        <v>0</v>
+      </c>
+      <c r="E54" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="12">
         <v>5</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B55" s="10">
         <v>47</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C55" s="10">
         <v>9</v>
       </c>
-      <c r="D55" s="5">
-        <v>0</v>
-      </c>
-      <c r="E55" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="10"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="10"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
+      <c r="D55" s="10">
+        <v>0</v>
+      </c>
+      <c r="E55" s="10">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1430,7 +1443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8391D5B3-C9B6-704C-A5E0-4930F20AA378}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="212" zoomScaleNormal="212" workbookViewId="0">
+    <sheetView zoomScale="212" zoomScaleNormal="212" workbookViewId="0">
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
@@ -1460,7 +1473,7 @@
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="11"/>
+      <c r="F1" s="3"/>
       <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1469,14 +1482,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1485,7 +1498,7 @@
       <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="1">
@@ -1494,7 +1507,7 @@
       <c r="E3" s="1">
         <v>63</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="1">
         <v>32</v>
       </c>
@@ -1516,7 +1529,7 @@
       <c r="E4" s="1">
         <v>62</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="1">
         <v>33</v>
       </c>
@@ -1538,7 +1551,7 @@
       <c r="E5" s="1">
         <v>61</v>
       </c>
-      <c r="F5" s="11"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="1">
         <v>34</v>
       </c>
@@ -1560,7 +1573,7 @@
       <c r="E6" s="1">
         <v>60</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="1">
         <v>35</v>
       </c>
@@ -1582,7 +1595,7 @@
       <c r="E7" s="1">
         <v>59</v>
       </c>
-      <c r="F7" s="11"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="1">
         <v>36</v>
       </c>
@@ -1603,7 +1616,7 @@
       <c r="E8" s="1">
         <v>58</v>
       </c>
-      <c r="F8" s="11"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="1">
         <v>37</v>
       </c>
@@ -1624,7 +1637,7 @@
       <c r="E9" s="1">
         <v>57</v>
       </c>
-      <c r="F9" s="11"/>
+      <c r="F9" s="3"/>
       <c r="G9" s="1">
         <v>38</v>
       </c>
@@ -1645,7 +1658,7 @@
       <c r="E10" s="1">
         <v>56</v>
       </c>
-      <c r="F10" s="11"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="1">
         <v>39</v>
       </c>
@@ -1666,7 +1679,7 @@
       <c r="E11" s="1">
         <v>55</v>
       </c>
-      <c r="F11" s="11"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="1">
         <v>40</v>
       </c>
@@ -1687,7 +1700,7 @@
       <c r="E12" s="1">
         <v>54</v>
       </c>
-      <c r="F12" s="11"/>
+      <c r="F12" s="3"/>
       <c r="G12" s="1">
         <v>41</v>
       </c>
@@ -1708,7 +1721,7 @@
       <c r="E13" s="1">
         <v>53</v>
       </c>
-      <c r="F13" s="11"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="1">
         <v>42</v>
       </c>
@@ -1729,7 +1742,7 @@
       <c r="E14" s="1">
         <v>52</v>
       </c>
-      <c r="F14" s="11"/>
+      <c r="F14" s="3"/>
       <c r="G14" s="1">
         <v>43</v>
       </c>
@@ -1750,7 +1763,7 @@
       <c r="E15" s="1">
         <v>51</v>
       </c>
-      <c r="F15" s="11"/>
+      <c r="F15" s="3"/>
       <c r="G15" s="1">
         <v>44</v>
       </c>
@@ -1771,7 +1784,7 @@
       <c r="E16" s="1">
         <v>50</v>
       </c>
-      <c r="F16" s="11"/>
+      <c r="F16" s="3"/>
       <c r="G16" s="1">
         <v>45</v>
       </c>
@@ -1792,7 +1805,7 @@
       <c r="E17" s="1">
         <v>49</v>
       </c>
-      <c r="F17" s="11"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="1">
         <v>46</v>
       </c>
@@ -1813,7 +1826,7 @@
       <c r="E18" s="1">
         <v>48</v>
       </c>
-      <c r="F18" s="11"/>
+      <c r="F18" s="3"/>
       <c r="G18" s="1">
         <v>47</v>
       </c>
@@ -1834,7 +1847,7 @@
       <c r="E19" s="1">
         <v>47</v>
       </c>
-      <c r="F19" s="11"/>
+      <c r="F19" s="3"/>
       <c r="G19" s="1">
         <v>48</v>
       </c>
@@ -1855,7 +1868,7 @@
       <c r="E20" s="1">
         <v>46</v>
       </c>
-      <c r="F20" s="11"/>
+      <c r="F20" s="3"/>
       <c r="G20" s="1">
         <v>49</v>
       </c>
@@ -1876,7 +1889,7 @@
       <c r="E21" s="1">
         <v>45</v>
       </c>
-      <c r="F21" s="11"/>
+      <c r="F21" s="3"/>
       <c r="G21" s="1">
         <v>50</v>
       </c>
@@ -1897,7 +1910,7 @@
       <c r="E22" s="1">
         <v>44</v>
       </c>
-      <c r="F22" s="11"/>
+      <c r="F22" s="3"/>
       <c r="G22" s="1">
         <v>51</v>
       </c>
@@ -1918,7 +1931,7 @@
       <c r="E23" s="1">
         <v>43</v>
       </c>
-      <c r="F23" s="11"/>
+      <c r="F23" s="3"/>
       <c r="G23" s="1">
         <v>52</v>
       </c>
@@ -1939,7 +1952,7 @@
       <c r="E24" s="1">
         <v>42</v>
       </c>
-      <c r="F24" s="11"/>
+      <c r="F24" s="3"/>
       <c r="G24" s="1">
         <v>53</v>
       </c>
@@ -1960,7 +1973,7 @@
       <c r="E25" s="1">
         <v>41</v>
       </c>
-      <c r="F25" s="11"/>
+      <c r="F25" s="3"/>
       <c r="G25" s="1">
         <v>54</v>
       </c>
@@ -1981,7 +1994,7 @@
       <c r="E26" s="1">
         <v>40</v>
       </c>
-      <c r="F26" s="11"/>
+      <c r="F26" s="3"/>
       <c r="G26" s="1">
         <v>55</v>
       </c>
@@ -2002,7 +2015,7 @@
       <c r="E27" s="1">
         <v>39</v>
       </c>
-      <c r="F27" s="11"/>
+      <c r="F27" s="3"/>
       <c r="G27" s="1">
         <v>56</v>
       </c>
@@ -2023,7 +2036,7 @@
       <c r="E28" s="1">
         <v>38</v>
       </c>
-      <c r="F28" s="11"/>
+      <c r="F28" s="3"/>
       <c r="G28" s="1">
         <v>57</v>
       </c>
@@ -2044,7 +2057,7 @@
       <c r="E29" s="1">
         <v>37</v>
       </c>
-      <c r="F29" s="11"/>
+      <c r="F29" s="3"/>
       <c r="G29" s="1">
         <v>58</v>
       </c>
@@ -2065,7 +2078,7 @@
       <c r="E30" s="1">
         <v>36</v>
       </c>
-      <c r="F30" s="11"/>
+      <c r="F30" s="3"/>
       <c r="G30" s="1">
         <v>59</v>
       </c>
@@ -2086,7 +2099,7 @@
       <c r="E31" s="1">
         <v>35</v>
       </c>
-      <c r="F31" s="11"/>
+      <c r="F31" s="3"/>
       <c r="G31" s="1">
         <v>60</v>
       </c>
@@ -2107,7 +2120,7 @@
       <c r="E32" s="1">
         <v>34</v>
       </c>
-      <c r="F32" s="11"/>
+      <c r="F32" s="3"/>
       <c r="G32" s="1">
         <v>61</v>
       </c>
@@ -2128,7 +2141,7 @@
       <c r="E33" s="1">
         <v>33</v>
       </c>
-      <c r="F33" s="11"/>
+      <c r="F33" s="3"/>
       <c r="G33" s="1">
         <v>62</v>
       </c>
@@ -2149,18 +2162,811 @@
       <c r="E34" s="1">
         <v>32</v>
       </c>
-      <c r="F34" s="11"/>
+      <c r="F34" s="3"/>
       <c r="G34" s="1">
         <v>63</v>
       </c>
       <c r="H34" s="1">
         <v>0</v>
       </c>
-      <c r="I34" s="13" t="s">
+      <c r="I34" s="5" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AC3C375-9CF0-4C49-9E4D-BF5081F2A73E}">
+  <dimension ref="A1:D55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="9.33203125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="13" style="15" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="15" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="42" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="17">
+        <v>0</v>
+      </c>
+      <c r="B3" s="18">
+        <v>0</v>
+      </c>
+      <c r="C3" s="19">
+        <v>0</v>
+      </c>
+      <c r="D3" s="19">
+        <f>C3+31</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="17">
+        <v>0</v>
+      </c>
+      <c r="B4" s="18">
+        <v>1</v>
+      </c>
+      <c r="C4" s="19">
+        <v>32</v>
+      </c>
+      <c r="D4" s="19">
+        <f t="shared" ref="D4:D55" si="0">C4+31</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="17">
+        <v>0</v>
+      </c>
+      <c r="B5" s="18">
+        <v>2</v>
+      </c>
+      <c r="C5" s="19">
+        <v>64</v>
+      </c>
+      <c r="D5" s="19">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="17">
+        <v>0</v>
+      </c>
+      <c r="B6" s="18">
+        <v>3</v>
+      </c>
+      <c r="C6" s="19">
+        <v>96</v>
+      </c>
+      <c r="D6" s="19">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="17">
+        <v>0</v>
+      </c>
+      <c r="B7" s="18">
+        <v>4</v>
+      </c>
+      <c r="C7" s="19">
+        <v>128</v>
+      </c>
+      <c r="D7" s="19">
+        <f t="shared" si="0"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="17">
+        <v>0</v>
+      </c>
+      <c r="B8" s="20">
+        <v>5</v>
+      </c>
+      <c r="C8" s="19">
+        <v>160</v>
+      </c>
+      <c r="D8" s="19">
+        <f t="shared" si="0"/>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="17">
+        <v>0</v>
+      </c>
+      <c r="B9" s="20">
+        <v>6</v>
+      </c>
+      <c r="C9" s="19">
+        <v>192</v>
+      </c>
+      <c r="D9" s="19">
+        <f t="shared" si="0"/>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="17">
+        <v>0</v>
+      </c>
+      <c r="B10" s="20">
+        <v>7</v>
+      </c>
+      <c r="C10" s="19">
+        <v>224</v>
+      </c>
+      <c r="D10" s="19">
+        <f t="shared" si="0"/>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="21">
+        <v>1</v>
+      </c>
+      <c r="B12" s="20">
+        <v>8</v>
+      </c>
+      <c r="C12" s="19">
+        <v>256</v>
+      </c>
+      <c r="D12" s="19">
+        <f t="shared" si="0"/>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="21">
+        <v>1</v>
+      </c>
+      <c r="B13" s="20">
+        <v>9</v>
+      </c>
+      <c r="C13" s="19">
+        <v>288</v>
+      </c>
+      <c r="D13" s="19">
+        <f t="shared" si="0"/>
+        <v>319</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="21">
+        <v>1</v>
+      </c>
+      <c r="B14" s="18">
+        <v>10</v>
+      </c>
+      <c r="C14" s="19">
+        <v>320</v>
+      </c>
+      <c r="D14" s="19">
+        <f t="shared" si="0"/>
+        <v>351</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="21">
+        <v>1</v>
+      </c>
+      <c r="B15" s="18">
+        <v>11</v>
+      </c>
+      <c r="C15" s="19">
+        <v>352</v>
+      </c>
+      <c r="D15" s="19">
+        <f t="shared" si="0"/>
+        <v>383</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="21">
+        <v>1</v>
+      </c>
+      <c r="B16" s="18">
+        <v>12</v>
+      </c>
+      <c r="C16" s="19">
+        <v>384</v>
+      </c>
+      <c r="D16" s="19">
+        <f t="shared" si="0"/>
+        <v>415</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="21">
+        <v>1</v>
+      </c>
+      <c r="B17" s="18">
+        <v>13</v>
+      </c>
+      <c r="C17" s="19">
+        <v>416</v>
+      </c>
+      <c r="D17" s="19">
+        <f t="shared" si="0"/>
+        <v>447</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="21">
+        <v>1</v>
+      </c>
+      <c r="B18" s="18">
+        <v>14</v>
+      </c>
+      <c r="C18" s="19">
+        <v>448</v>
+      </c>
+      <c r="D18" s="19">
+        <f t="shared" si="0"/>
+        <v>479</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="21">
+        <v>1</v>
+      </c>
+      <c r="B19" s="20">
+        <v>15</v>
+      </c>
+      <c r="C19" s="19">
+        <v>480</v>
+      </c>
+      <c r="D19" s="19">
+        <f t="shared" si="0"/>
+        <v>511</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="17">
+        <v>2</v>
+      </c>
+      <c r="B21" s="20">
+        <v>16</v>
+      </c>
+      <c r="C21" s="19">
+        <v>512</v>
+      </c>
+      <c r="D21" s="19">
+        <f t="shared" si="0"/>
+        <v>543</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="17">
+        <v>2</v>
+      </c>
+      <c r="B22" s="20">
+        <v>17</v>
+      </c>
+      <c r="C22" s="19">
+        <v>544</v>
+      </c>
+      <c r="D22" s="19">
+        <f t="shared" si="0"/>
+        <v>575</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="17">
+        <v>2</v>
+      </c>
+      <c r="B23" s="20">
+        <v>18</v>
+      </c>
+      <c r="C23" s="19">
+        <v>576</v>
+      </c>
+      <c r="D23" s="19">
+        <f t="shared" si="0"/>
+        <v>607</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="17">
+        <v>2</v>
+      </c>
+      <c r="B24" s="20">
+        <v>19</v>
+      </c>
+      <c r="C24" s="19">
+        <v>608</v>
+      </c>
+      <c r="D24" s="19">
+        <f t="shared" si="0"/>
+        <v>639</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="17">
+        <v>2</v>
+      </c>
+      <c r="B25" s="18">
+        <v>20</v>
+      </c>
+      <c r="C25" s="19">
+        <v>640</v>
+      </c>
+      <c r="D25" s="19">
+        <f t="shared" si="0"/>
+        <v>671</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="17">
+        <v>2</v>
+      </c>
+      <c r="B26" s="18">
+        <v>21</v>
+      </c>
+      <c r="C26" s="19">
+        <v>672</v>
+      </c>
+      <c r="D26" s="19">
+        <f t="shared" si="0"/>
+        <v>703</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="17">
+        <v>2</v>
+      </c>
+      <c r="B27" s="18">
+        <v>22</v>
+      </c>
+      <c r="C27" s="19">
+        <v>704</v>
+      </c>
+      <c r="D27" s="19">
+        <f t="shared" si="0"/>
+        <v>735</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="17">
+        <v>2</v>
+      </c>
+      <c r="B28" s="18">
+        <v>23</v>
+      </c>
+      <c r="C28" s="19">
+        <v>736</v>
+      </c>
+      <c r="D28" s="19">
+        <f t="shared" si="0"/>
+        <v>767</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="22">
+        <v>3</v>
+      </c>
+      <c r="B30" s="18">
+        <v>24</v>
+      </c>
+      <c r="C30" s="19">
+        <v>768</v>
+      </c>
+      <c r="D30" s="19">
+        <f t="shared" si="0"/>
+        <v>799</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="22">
+        <v>3</v>
+      </c>
+      <c r="B31" s="20">
+        <v>25</v>
+      </c>
+      <c r="C31" s="19">
+        <v>800</v>
+      </c>
+      <c r="D31" s="19">
+        <f t="shared" si="0"/>
+        <v>831</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="22">
+        <v>3</v>
+      </c>
+      <c r="B32" s="20">
+        <v>26</v>
+      </c>
+      <c r="C32" s="19">
+        <v>832</v>
+      </c>
+      <c r="D32" s="19">
+        <f t="shared" si="0"/>
+        <v>863</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="22">
+        <v>3</v>
+      </c>
+      <c r="B33" s="20">
+        <v>27</v>
+      </c>
+      <c r="C33" s="19">
+        <v>864</v>
+      </c>
+      <c r="D33" s="19">
+        <f t="shared" si="0"/>
+        <v>895</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="22">
+        <v>3</v>
+      </c>
+      <c r="B34" s="20">
+        <v>28</v>
+      </c>
+      <c r="C34" s="19">
+        <v>896</v>
+      </c>
+      <c r="D34" s="19">
+        <f t="shared" si="0"/>
+        <v>927</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="22">
+        <v>3</v>
+      </c>
+      <c r="B35" s="20">
+        <v>29</v>
+      </c>
+      <c r="C35" s="19">
+        <v>928</v>
+      </c>
+      <c r="D35" s="19">
+        <f t="shared" si="0"/>
+        <v>959</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="22">
+        <v>3</v>
+      </c>
+      <c r="B36" s="18">
+        <v>30</v>
+      </c>
+      <c r="C36" s="19">
+        <v>960</v>
+      </c>
+      <c r="D36" s="19">
+        <f t="shared" si="0"/>
+        <v>991</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="22">
+        <v>3</v>
+      </c>
+      <c r="B37" s="18">
+        <v>31</v>
+      </c>
+      <c r="C37" s="19">
+        <v>992</v>
+      </c>
+      <c r="D37" s="19">
+        <f t="shared" si="0"/>
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="17">
+        <v>4</v>
+      </c>
+      <c r="B39" s="18">
+        <v>32</v>
+      </c>
+      <c r="C39" s="19">
+        <v>1024</v>
+      </c>
+      <c r="D39" s="19">
+        <f t="shared" si="0"/>
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="17">
+        <v>4</v>
+      </c>
+      <c r="B40" s="18">
+        <v>33</v>
+      </c>
+      <c r="C40" s="19">
+        <v>1056</v>
+      </c>
+      <c r="D40" s="19">
+        <f t="shared" si="0"/>
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="17">
+        <v>4</v>
+      </c>
+      <c r="B41" s="18">
+        <v>34</v>
+      </c>
+      <c r="C41" s="19">
+        <v>1088</v>
+      </c>
+      <c r="D41" s="19">
+        <f t="shared" si="0"/>
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="17">
+        <v>4</v>
+      </c>
+      <c r="B42" s="20">
+        <v>35</v>
+      </c>
+      <c r="C42" s="19">
+        <v>1120</v>
+      </c>
+      <c r="D42" s="19">
+        <f t="shared" si="0"/>
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="17">
+        <v>4</v>
+      </c>
+      <c r="B43" s="20">
+        <v>36</v>
+      </c>
+      <c r="C43" s="19">
+        <v>1152</v>
+      </c>
+      <c r="D43" s="19">
+        <f t="shared" si="0"/>
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="17">
+        <v>4</v>
+      </c>
+      <c r="B44" s="20">
+        <v>37</v>
+      </c>
+      <c r="C44" s="19">
+        <v>1184</v>
+      </c>
+      <c r="D44" s="19">
+        <f t="shared" si="0"/>
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="17">
+        <v>4</v>
+      </c>
+      <c r="B45" s="20">
+        <v>38</v>
+      </c>
+      <c r="C45" s="19">
+        <v>1216</v>
+      </c>
+      <c r="D45" s="19">
+        <f t="shared" si="0"/>
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="17">
+        <v>4</v>
+      </c>
+      <c r="B46" s="20">
+        <v>39</v>
+      </c>
+      <c r="C46" s="19">
+        <v>1248</v>
+      </c>
+      <c r="D46" s="19">
+        <f t="shared" si="0"/>
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="22">
+        <v>5</v>
+      </c>
+      <c r="B48" s="18">
+        <v>40</v>
+      </c>
+      <c r="C48" s="19">
+        <v>1280</v>
+      </c>
+      <c r="D48" s="19">
+        <f t="shared" si="0"/>
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="22">
+        <v>5</v>
+      </c>
+      <c r="B49" s="18">
+        <v>41</v>
+      </c>
+      <c r="C49" s="19">
+        <v>1312</v>
+      </c>
+      <c r="D49" s="19">
+        <f t="shared" si="0"/>
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="22">
+        <v>5</v>
+      </c>
+      <c r="B50" s="18">
+        <v>42</v>
+      </c>
+      <c r="C50" s="19">
+        <v>1344</v>
+      </c>
+      <c r="D50" s="19">
+        <f t="shared" si="0"/>
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="22">
+        <v>5</v>
+      </c>
+      <c r="B51" s="18">
+        <v>43</v>
+      </c>
+      <c r="C51" s="19">
+        <v>1376</v>
+      </c>
+      <c r="D51" s="19">
+        <f t="shared" si="0"/>
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="22">
+        <v>5</v>
+      </c>
+      <c r="B52" s="18">
+        <v>44</v>
+      </c>
+      <c r="C52" s="19">
+        <v>1408</v>
+      </c>
+      <c r="D52" s="19">
+        <f t="shared" si="0"/>
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="22">
+        <v>5</v>
+      </c>
+      <c r="B53" s="20">
+        <v>45</v>
+      </c>
+      <c r="C53" s="19">
+        <v>1440</v>
+      </c>
+      <c r="D53" s="19">
+        <f t="shared" si="0"/>
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="22">
+        <v>5</v>
+      </c>
+      <c r="B54" s="20">
+        <v>46</v>
+      </c>
+      <c r="C54" s="19">
+        <v>1472</v>
+      </c>
+      <c r="D54" s="19">
+        <f t="shared" si="0"/>
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="22">
+        <v>5</v>
+      </c>
+      <c r="B55" s="20">
+        <v>47</v>
+      </c>
+      <c r="C55" s="19">
+        <v>1504</v>
+      </c>
+      <c r="D55" s="19">
+        <f t="shared" si="0"/>
+        <v>1535</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>